<commit_message>
minor change in input file to correct mispelled words. Continuation of development of femfilegenerator.py.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771FFEAB-9775-4325-930D-8E8E85E18CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -269,32 +268,6 @@
   </si>
   <si>
     <t>Material Details</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A specification of the materials for each component. The naming scheme follows an A-B-C-D pattern. The material database can be found in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>materials.exe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and the patter is defined as specified on the right</t>
-    </r>
   </si>
   <si>
     <t>A:</t>
@@ -486,11 +459,37 @@
       <t xml:space="preserve">The trimming of the skin and ribs must be input also as a fraction of the chord. These last inputs are included so as to prevent issues with the NASTRAN tool. </t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A specification of the materials for each component. The naming scheme follows an A-B-C-D pattern. The material database can be found in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>materials.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and the pattern is defined as specified on the right</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1244,12 +1243,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,12 +1548,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,16 +1600,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="D4" s="31" t="s">
         <v>100</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>101</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -1686,7 +1685,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="11">
         <v>1000</v>
@@ -1713,12 +1712,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,7 +1734,7 @@
       <c r="C1" s="50"/>
       <c r="D1" s="51"/>
       <c r="E1" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="38"/>
       <c r="G1" s="38"/>
@@ -1873,17 +1872,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1917,7 +1916,7 @@
       <c r="C15" s="53"/>
       <c r="D15" s="54"/>
       <c r="E15" s="61" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
@@ -1927,10 +1926,10 @@
       <c r="K15" s="62"/>
       <c r="L15" s="63"/>
       <c r="M15" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N15" s="70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O15" s="70"/>
       <c r="P15" s="70"/>
@@ -1951,10 +1950,10 @@
       <c r="K16" s="65"/>
       <c r="L16" s="66"/>
       <c r="M16" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O16" s="43"/>
       <c r="P16" s="43"/>
@@ -1975,10 +1974,10 @@
       <c r="K17" s="65"/>
       <c r="L17" s="66"/>
       <c r="M17" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O17" s="43"/>
       <c r="P17" s="43"/>
@@ -1999,10 +1998,10 @@
       <c r="K18" s="68"/>
       <c r="L18" s="69"/>
       <c r="M18" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N18" s="45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O18" s="45"/>
       <c r="P18" s="45"/>
@@ -2012,13 +2011,13 @@
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="49"/>
       <c r="B20" s="47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="H20" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
@@ -2028,82 +2027,82 @@
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="H21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="J21" s="48" t="s">
         <v>72</v>
-      </c>
-      <c r="J21" s="48" t="s">
-        <v>73</v>
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="49"/>
       <c r="B22" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="16" t="s">
+      <c r="K22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="L22" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="D23" s="8">
         <v>1.27</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="J23">
         <v>0.20319999999999999</v>
@@ -2112,30 +2111,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
       </c>
       <c r="D24">
         <v>1.524</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J24">
         <v>0.20319999999999999</v>
@@ -2144,30 +2143,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
         <v>79</v>
-      </c>
-      <c r="C25" t="s">
-        <v>80</v>
       </c>
       <c r="D25">
         <v>1.27</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J25">
         <v>0.254</v>
@@ -2176,30 +2175,30 @@
         <v>1.5748</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
         <v>83</v>
-      </c>
-      <c r="C26" t="s">
-        <v>84</v>
       </c>
       <c r="D26">
         <v>1.524</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J26">
         <v>0.254</v>
@@ -2208,30 +2207,30 @@
         <v>1.5748</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
         <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
       </c>
       <c r="D27">
         <v>1.27</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J27">
         <v>1.6001999999999998</v>
@@ -2240,30 +2239,30 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="D28" s="12">
         <v>1.524</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J28">
         <v>1.6001999999999998</v>
@@ -2272,15 +2271,15 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J29">
         <v>3.2765999999999997</v>
@@ -2289,15 +2288,15 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J30">
         <v>3.2765999999999997</v>
@@ -2306,7 +2305,7 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2315,10 +2314,10 @@
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="H31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J31">
         <v>6.35</v>
@@ -2327,15 +2326,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J32">
         <v>6.35</v>
@@ -2344,15 +2343,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J33">
         <v>38.125399999999992</v>
@@ -2361,15 +2360,15 @@
         <v>50.8</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J34">
         <v>38.125399999999992</v>
@@ -2378,15 +2377,15 @@
         <v>50.8</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J35">
         <v>50.825399999999995</v>
@@ -2395,15 +2394,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J36">
         <v>50.825399999999995</v>
@@ -2412,15 +2411,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J37">
         <v>76.225399999999993</v>
@@ -2429,15 +2428,15 @@
         <v>101.6</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J38">
         <v>76.225399999999993</v>
@@ -2446,15 +2445,15 @@
         <v>101.6</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="J39">
         <v>1.016</v>
@@ -2463,15 +2462,15 @@
         <v>1.5748</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I40" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="J40">
         <v>1.6001999999999998</v>
@@ -2480,15 +2479,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="J41">
         <v>1.6001999999999998</v>
@@ -2497,15 +2496,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H42" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="J42" s="12">
         <v>4.7751999999999999</v>
@@ -2514,7 +2513,7 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2539,7 +2538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2551,13 +2550,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="51"/>
       <c r="E1" s="72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="73"/>
       <c r="G1" s="73"/>

</xml_diff>

<commit_message>
Fixed th AVL_analysis portion, reorganized the tree and the folders, corrected the avl inputs
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9ECE2D-972D-4D54-BCA8-E522C2B1EC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -268,6 +269,32 @@
   </si>
   <si>
     <t>Material Details</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A specification of the materials for each component. The naming scheme follows an A-B-C-D pattern. The material database can be found in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>materials.exe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and the patter is defined as specified on the right</t>
+    </r>
   </si>
   <si>
     <t>A:</t>
@@ -459,37 +486,11 @@
       <t xml:space="preserve">The trimming of the skin and ribs must be input also as a fraction of the chord. These last inputs are included so as to prevent issues with the NASTRAN tool. </t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A specification of the materials for each component. The naming scheme follows an A-B-C-D pattern. The material database can be found in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>materials.csv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and the pattern is defined as specified on the right</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -738,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -930,6 +931,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1243,12 +1248,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,12 +1553,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1600,16 +1605,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -1653,53 +1658,38 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="6">
-        <v>5000</v>
-      </c>
-      <c r="C7">
-        <v>5050</v>
-      </c>
-      <c r="D7">
-        <v>3000</v>
-      </c>
-      <c r="E7" s="8"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="6">
-        <v>80</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>40</v>
-      </c>
-      <c r="H8" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5000</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="11">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="4">
         <v>1000</v>
       </c>
-      <c r="C9" s="12">
-        <v>3500</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1712,12 +1702,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,7 +1724,7 @@
       <c r="C1" s="50"/>
       <c r="D1" s="51"/>
       <c r="E1" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F1" s="38"/>
       <c r="G1" s="38"/>
@@ -1872,17 +1862,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1916,7 +1906,7 @@
       <c r="C15" s="53"/>
       <c r="D15" s="54"/>
       <c r="E15" s="61" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
@@ -1926,10 +1916,10 @@
       <c r="K15" s="62"/>
       <c r="L15" s="63"/>
       <c r="M15" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N15" s="70" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O15" s="70"/>
       <c r="P15" s="70"/>
@@ -1950,10 +1940,10 @@
       <c r="K16" s="65"/>
       <c r="L16" s="66"/>
       <c r="M16" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O16" s="43"/>
       <c r="P16" s="43"/>
@@ -1974,10 +1964,10 @@
       <c r="K17" s="65"/>
       <c r="L17" s="66"/>
       <c r="M17" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O17" s="43"/>
       <c r="P17" s="43"/>
@@ -1998,10 +1988,10 @@
       <c r="K18" s="68"/>
       <c r="L18" s="69"/>
       <c r="M18" s="25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N18" s="45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O18" s="45"/>
       <c r="P18" s="45"/>
@@ -2011,13 +2001,13 @@
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="49"/>
       <c r="B20" s="47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="H20" s="47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
@@ -2027,82 +2017,82 @@
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="I21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="J21" s="48" t="s">
         <v>73</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J21" s="48" t="s">
-        <v>72</v>
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="49"/>
       <c r="B22" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E22" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>76</v>
-      </c>
       <c r="L22" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D23" s="8">
         <v>1.27</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J23">
         <v>0.20319999999999999</v>
@@ -2111,30 +2101,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24">
         <v>1.524</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J24">
         <v>0.20319999999999999</v>
@@ -2143,30 +2133,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25">
         <v>1.27</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J25">
         <v>0.254</v>
@@ -2175,30 +2165,30 @@
         <v>1.5748</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>1.524</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J26">
         <v>0.254</v>
@@ -2207,30 +2197,30 @@
         <v>1.5748</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D27">
         <v>1.27</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J27">
         <v>1.6001999999999998</v>
@@ -2239,30 +2229,30 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" s="12">
         <v>1.524</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J28">
         <v>1.6001999999999998</v>
@@ -2271,15 +2261,15 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H29" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J29">
         <v>3.2765999999999997</v>
@@ -2288,15 +2278,15 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H30" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J30">
         <v>3.2765999999999997</v>
@@ -2305,7 +2295,7 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2314,10 +2304,10 @@
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="H31" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J31">
         <v>6.35</v>
@@ -2326,15 +2316,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H32" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J32">
         <v>6.35</v>
@@ -2343,15 +2333,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H33" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J33">
         <v>38.125399999999992</v>
@@ -2360,15 +2350,15 @@
         <v>50.8</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H34" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J34">
         <v>38.125399999999992</v>
@@ -2377,15 +2367,15 @@
         <v>50.8</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H35" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J35">
         <v>50.825399999999995</v>
@@ -2394,15 +2384,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H36" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J36">
         <v>50.825399999999995</v>
@@ -2411,15 +2401,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H37" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J37">
         <v>76.225399999999993</v>
@@ -2428,15 +2418,15 @@
         <v>101.6</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H38" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J38">
         <v>76.225399999999993</v>
@@ -2445,15 +2435,15 @@
         <v>101.6</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H39" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J39">
         <v>1.016</v>
@@ -2462,15 +2452,15 @@
         <v>1.5748</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H40" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J40">
         <v>1.6001999999999998</v>
@@ -2479,15 +2469,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H41" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J41">
         <v>1.6001999999999998</v>
@@ -2496,15 +2486,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H42" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J42" s="12">
         <v>4.7751999999999999</v>
@@ -2513,7 +2503,7 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2538,25 +2528,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E1" sqref="E1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="51"/>
       <c r="E1" s="72" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" s="73"/>
       <c r="G1" s="73"/>

</xml_diff>

<commit_message>
Introduced a lot of warning messages in the initialization file
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9ECE2D-972D-4D54-BCA8-E522C2B1EC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BB21AB-E633-49DB-A40B-2D46F2E0D909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,6 +554,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -768,9 +774,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -808,6 +811,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -931,10 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,10 +1259,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,22 +1273,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1434,22 +1443,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="41"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
@@ -1490,41 +1499,41 @@
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18">
+        <v>14013</v>
+      </c>
+      <c r="D18" s="18">
+        <v>2412</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="19">
-        <v>2412</v>
-      </c>
-      <c r="E18" s="19">
-        <v>14013</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="77">
         <v>0</v>
       </c>
-      <c r="C19" s="12">
-        <v>0.3</v>
+      <c r="C19" s="77">
+        <v>1</v>
       </c>
       <c r="D19" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="12">
         <v>0.7</v>
-      </c>
-      <c r="E19" s="12">
-        <v>1</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -1533,11 +1542,6 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="13"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I22">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1557,8 +1561,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1567,18 +1571,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -1607,37 +1611,37 @@
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1658,14 +1662,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="10"/>
+      <c r="C7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1706,8 +1703,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,28 +1714,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1816,7 +1813,7 @@
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="20"/>
       <c r="C6">
         <v>7</v>
       </c>
@@ -1832,12 +1829,12 @@
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="20"/>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1848,7 +1845,7 @@
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8">
         <v>5</v>
       </c>
@@ -1864,14 +1861,14 @@
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>103</v>
       </c>
       <c r="F9" s="12"/>
@@ -1899,123 +1896,123 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="61" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="23" t="s">
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="N15" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="70"/>
-      <c r="R15" s="71"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="73"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="24" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="43" t="s">
+      <c r="N16" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="44"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="46"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="24" t="s">
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="N17" s="43" t="s">
+      <c r="N17" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="44"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="46"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="25" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="45" t="s">
+      <c r="N18" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="46"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="48"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="51"/>
+      <c r="B20" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="H20" s="47" t="s">
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="H20" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="16" t="s">
         <v>71</v>
       </c>
@@ -2034,26 +2031,26 @@
       <c r="I21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="48"/>
+      <c r="K21" s="50"/>
       <c r="L21" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="26" t="s">
         <v>78</v>
       </c>
       <c r="H22" s="16" t="s">
@@ -2073,7 +2070,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="25" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2105,7 +2102,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>89</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -2137,7 +2134,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -2169,7 +2166,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>91</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -2201,7 +2198,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>93</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -2233,7 +2230,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="25" t="s">
         <v>94</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -2299,10 +2296,10 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
       <c r="H31" s="6" t="s">
         <v>81</v>
       </c>
@@ -2539,19 +2536,19 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="72" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="74"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changed spar, rib, and stringer rules. Better performance in all of them
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFAF25E-2156-43E2-9476-15ED41F27A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686D06D1-3CD8-4EEE-9B9D-EF4EE06FE006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1561,8 +1561,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1703,7 +1703,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finally fixed the spar placement
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B15F20B-B401-49AF-9505-8BF54D3226E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F16F4D1-AE25-4184-A3A1-123DE20B5EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="12">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E19" s="12">
         <v>0.8125</v>
@@ -1704,7 +1704,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1778,13 +1778,13 @@
         <v>53</v>
       </c>
       <c r="B4">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="D4">
-        <v>0.21</v>
+        <v>0.05</v>
       </c>
       <c r="E4">
         <v>0.2</v>

</xml_diff>

<commit_message>
Fixed STEP file writing.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F16F4D1-AE25-4184-A3A1-123DE20B5EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -397,9 +396,6 @@
   </si>
   <si>
     <t>Here, the number of FEM elements and boundary conditions are specified</t>
-  </si>
-  <si>
-    <t>Flight Altitude [m]</t>
   </si>
   <si>
     <t>Case name</t>
@@ -486,11 +482,14 @@
       <t xml:space="preserve">The trimming of the skin and ribs must be input also as a fraction of the chord. These last inputs are included so as to prevent issues with the NASTRAN tool. </t>
     </r>
   </si>
+  <si>
+    <t>Flight Altitude [ft]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -820,6 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,7 +943,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,12 +1256,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,22 +1272,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1443,22 +1442,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
@@ -1523,14 +1522,14 @@
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="77">
+      <c r="B19" s="36">
         <v>0</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="36">
         <v>1</v>
       </c>
       <c r="D19" s="12">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="12">
         <v>0.8125</v>
@@ -1557,12 +1556,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,18 +1570,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -1609,16 +1608,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
@@ -1682,7 +1681,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B10" s="4">
         <v>1000</v>
@@ -1699,12 +1698,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,28 +1713,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="41"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1778,16 +1777,16 @@
         <v>53</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D4">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="L4" s="10"/>
     </row>
@@ -1799,13 +1798,13 @@
         <v>0.75</v>
       </c>
       <c r="C5">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="D5">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -1859,17 +1858,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1896,123 +1895,123 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="63" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66"/>
       <c r="M15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="N15" s="72" t="s">
+      <c r="N15" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="74"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="68"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="69"/>
       <c r="M16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="45" t="s">
+      <c r="N16" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="68"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="69"/>
       <c r="M17" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="N17" s="45" t="s">
+      <c r="N17" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="71"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="72"/>
       <c r="M18" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="47" t="s">
+      <c r="N18" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="49"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="49" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="H20" s="49" t="s">
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="H20" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="16" t="s">
         <v>71</v>
       </c>
@@ -2031,16 +2030,16 @@
       <c r="I21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="50" t="s">
+      <c r="J21" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="50"/>
+      <c r="K21" s="51"/>
       <c r="L21" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="26" t="s">
         <v>75</v>
       </c>
@@ -2296,10 +2295,10 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
       <c r="H31" s="6" t="s">
         <v>81</v>
       </c>
@@ -2525,7 +2524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -2536,19 +2535,19 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="74" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
changes in the input file and airfoils
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F16F4D1-AE25-4184-A3A1-123DE20B5EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210F75D-4BE0-423E-8967-94B9A8FE54FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="122">
   <si>
     <t>Section 1</t>
   </si>
@@ -102,9 +102,6 @@
     <t>rae5212</t>
   </si>
   <si>
-    <t>whitcomb</t>
-  </si>
-  <si>
     <t>Section 11</t>
   </si>
   <si>
@@ -127,64 +124,6 @@
   </si>
   <si>
     <t>CL</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Airfoils can be specified as NACA 4/5 digit airfoils, or through the name from its respective </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.dat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> file in the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>airfoil</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> folder. The position is specified between 0 and 1 as a percentage of the half-span. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Root and tip airfoils are required.</t>
-    </r>
   </si>
   <si>
     <t>Airfoil 1</t>
@@ -485,6 +424,175 @@
       </rPr>
       <t xml:space="preserve">The trimming of the skin and ribs must be input also as a fraction of the chord. These last inputs are included so as to prevent issues with the NASTRAN tool. </t>
     </r>
+  </si>
+  <si>
+    <t>rae5215</t>
+  </si>
+  <si>
+    <t>Possible Non-NACA Airfoils</t>
+  </si>
+  <si>
+    <t>B29_root</t>
+  </si>
+  <si>
+    <t>B29_tip</t>
+  </si>
+  <si>
+    <t>B707_root</t>
+  </si>
+  <si>
+    <t>B707_tip</t>
+  </si>
+  <si>
+    <t>B707_54c</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Naca 4 Digit (ABCC):                             </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Naca 5 Digit (ABBCC):                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Max camber (A = x/c %)            </t>
+  </si>
+  <si>
+    <t>B: Max camber location  (B*10 = x/c %)</t>
+  </si>
+  <si>
+    <t>C: Max thickness location (C = x/c %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Design CL (A = 3/2 * CL_des)            </t>
+  </si>
+  <si>
+    <t>B: Max camber location (B = 2* x/c %)</t>
+  </si>
+  <si>
+    <t>Root and tip airfoils are required.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Airfoils can be specified as NACA 4/5 digit airfoils, or through the name from its respective </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.dat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file in the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>airfoil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder. The position is specified between 0 and 1 as a percentage of the half-span.              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If you want to upload your own airfoils, add its</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .dat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wingbox_code/input_data/airfoil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>rae2822</t>
+  </si>
+  <si>
+    <t>SC2-0714</t>
   </si>
 </sst>
 </file>
@@ -745,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -820,6 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,7 +1052,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,49 +1411,62 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
+    <col min="15" max="15" width="16.77734375" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="14" t="s">
         <v>0</v>
@@ -1350,10 +1515,10 @@
         <v>9</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1375,7 +1540,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1555,7 @@
       </c>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1570,7 @@
       </c>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1585,7 @@
       </c>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1442,113 +1607,246 @@
       <c r="K12" s="12"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="15" spans="1:12" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="N15" s="88"/>
+      <c r="O15" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="P15" s="88"/>
+    </row>
+    <row r="16" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="58"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="83" t="s">
+        <v>112</v>
+      </c>
+      <c r="N16" s="84"/>
+      <c r="O16" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="P16" s="84"/>
+    </row>
+    <row r="17" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="58"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="N17" s="84"/>
+      <c r="O17" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="P17" s="84"/>
+    </row>
+    <row r="18" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="70" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="N18" s="86"/>
+      <c r="O18" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="P18" s="86"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="G20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="H20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="K20" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="L20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="N20" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="O20" s="92"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="78"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="N21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="36">
+        <v>0</v>
+      </c>
+      <c r="C22" s="36">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0.54</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="13"/>
+      <c r="N22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O22" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="18">
-        <v>14013</v>
-      </c>
-      <c r="D18" s="18">
-        <v>2412</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="77">
-        <v>0</v>
-      </c>
-      <c r="C19" s="77">
-        <v>1</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0.8125</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
+      <c r="P22" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M25" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="15">
+    <mergeCell ref="E15:L16"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A15:D15"/>
     <mergeCell ref="E1:L1"/>
-    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1571,54 +1869,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="A1" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
@@ -1627,16 +1925,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>32</v>
-      </c>
       <c r="D5" s="34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
@@ -1645,7 +1943,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="11">
         <v>3</v>
@@ -1666,7 +1964,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>5000</v>
@@ -1674,7 +1972,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="7">
         <v>80</v>
@@ -1682,7 +1980,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4">
         <v>1000</v>
@@ -1714,28 +2012,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="41"/>
+      <c r="A1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1775,7 +2073,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>0.05</v>
@@ -1793,7 +2091,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0.75</v>
@@ -1811,7 +2109,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6">
@@ -1827,7 +2125,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7">
@@ -1843,7 +2141,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8">
@@ -1859,17 +2157,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1881,7 +2179,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3">
         <v>0.94</v>
@@ -1889,207 +2187,207 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" s="4">
         <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="63" t="s">
+      <c r="N15" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="74"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="22" t="s">
+      <c r="N16" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N15" s="72" t="s">
+      <c r="N17" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="73"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="23" t="s">
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="45" t="s">
+      <c r="N18" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="46"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="N17" s="45" t="s">
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="49"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="H20" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="46"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="24" t="s">
+      <c r="C21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="51"/>
+      <c r="L21" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="52"/>
+      <c r="B22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="48"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="H20" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="D22" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="I22" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" s="50"/>
-      <c r="L21" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="26" t="s">
+      <c r="K22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="16" t="s">
+      <c r="L22" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" s="8">
         <v>1.27</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J23">
         <v>0.20319999999999999</v>
@@ -2098,30 +2396,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>1.524</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J24">
         <v>0.20319999999999999</v>
@@ -2130,30 +2428,30 @@
         <v>0.22859999999999997</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>1.27</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J25">
         <v>0.254</v>
@@ -2162,30 +2460,30 @@
         <v>1.5748</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26">
         <v>1.524</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J26">
         <v>0.254</v>
@@ -2194,30 +2492,30 @@
         <v>1.5748</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27">
         <v>1.27</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J27">
         <v>1.6001999999999998</v>
@@ -2226,30 +2524,30 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="12">
         <v>1.524</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J28">
         <v>1.6001999999999998</v>
@@ -2258,15 +2556,15 @@
         <v>3.2511999999999999</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H29" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J29">
         <v>3.2765999999999997</v>
@@ -2275,15 +2573,15 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H30" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J30">
         <v>3.2765999999999997</v>
@@ -2292,19 +2590,19 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
       <c r="H31" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J31">
         <v>6.35</v>
@@ -2313,15 +2611,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H32" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J32">
         <v>6.35</v>
@@ -2330,15 +2628,15 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H33" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J33">
         <v>38.125399999999992</v>
@@ -2347,15 +2645,15 @@
         <v>50.8</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H34" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J34">
         <v>38.125399999999992</v>
@@ -2364,15 +2662,15 @@
         <v>50.8</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H35" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J35">
         <v>50.825399999999995</v>
@@ -2381,15 +2679,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H36" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J36">
         <v>50.825399999999995</v>
@@ -2398,15 +2696,15 @@
         <v>76.199999999999989</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H37" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J37">
         <v>76.225399999999993</v>
@@ -2415,15 +2713,15 @@
         <v>101.6</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H38" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J38">
         <v>76.225399999999993</v>
@@ -2432,15 +2730,15 @@
         <v>101.6</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H39" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J39">
         <v>1.016</v>
@@ -2449,15 +2747,15 @@
         <v>1.5748</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H40" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J40">
         <v>1.6001999999999998</v>
@@ -2466,15 +2764,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H41" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J41">
         <v>1.6001999999999998</v>
@@ -2483,15 +2781,15 @@
         <v>4.7497999999999996</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H42" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J42" s="12">
         <v>4.7751999999999999</v>
@@ -2500,7 +2798,7 @@
         <v>6.3245999999999993</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2536,19 +2834,19 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
+      <c r="A1" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added validators for the geometry, loads and structure inputs
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428BB5A2-3ED4-4AD3-AF7D-9EB8633132DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB36DF-B06D-49A3-B3FC-B5BE64775044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -929,6 +929,72 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -938,15 +1004,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -964,66 +1024,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1393,8 +1393,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,22 +1418,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="56"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1588,100 +1588,100 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="37" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="49" t="s">
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="50"/>
-      <c r="O15" s="49" t="s">
+      <c r="N15" s="56"/>
+      <c r="O15" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="P15" s="50"/>
+      <c r="P15" s="56"/>
     </row>
     <row r="16" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="40" t="s">
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="40" t="s">
+      <c r="N16" s="58"/>
+      <c r="O16" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="P16" s="42"/>
+      <c r="P16" s="58"/>
     </row>
     <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="43" t="s">
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="40" t="s">
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="N17" s="42"/>
-      <c r="O17" s="40" t="s">
+      <c r="N17" s="58"/>
+      <c r="O17" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="P17" s="42"/>
+      <c r="P17" s="58"/>
     </row>
     <row r="18" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="46" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="46" t="s">
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="N18" s="48"/>
-      <c r="O18" s="46" t="s">
+      <c r="N18" s="68"/>
+      <c r="O18" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="P18" s="48"/>
+      <c r="P18" s="68"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
@@ -1717,11 +1717,11 @@
       <c r="L20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="N20" s="57" t="s">
+      <c r="N20" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="O20" s="58"/>
-      <c r="P20" s="59"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="45"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1829,7 +1829,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1839,18 +1839,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="70"/>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="56"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -1982,28 +1982,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
       <c r="D1" s="80"/>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="56"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -2164,22 +2164,22 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="37" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="61"/>
       <c r="M15" s="22" t="s">
         <v>61</v>
       </c>
@@ -2192,18 +2192,18 @@
       <c r="R15" s="82"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="58"/>
       <c r="M16" s="23" t="s">
         <v>62</v>
       </c>
@@ -2216,18 +2216,18 @@
       <c r="R16" s="73"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="58"/>
       <c r="M17" s="23" t="s">
         <v>63</v>
       </c>
@@ -2240,18 +2240,18 @@
       <c r="R17" s="73"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="68"/>
       <c r="M18" s="24" t="s">
         <v>64</v>
       </c>
@@ -2804,7 +2804,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="79"/>

</xml_diff>

<commit_message>
Minor changes to femfilegenerator.py
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB36DF-B06D-49A3-B3FC-B5BE64775044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -598,7 +597,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1389,12 +1388,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1728,16 +1727,16 @@
         <v>22</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -1825,7 +1824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -1967,12 +1966,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2046,16 +2045,16 @@
         <v>51</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D4">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="L4" s="10"/>
     </row>
@@ -2067,13 +2066,13 @@
         <v>0.75</v>
       </c>
       <c r="C5">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="D5">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -2793,7 +2792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Final commit before rollback
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB36DF-B06D-49A3-B3FC-B5BE64775044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6698AA14-F0B7-4507-BE9C-EA5A78867782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
   <si>
     <t>Section 1</t>
   </si>
@@ -350,79 +350,6 @@
     <t>cl_high</t>
   </si>
   <si>
-    <t>Stringer Cross-section</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The front and rear spar locations must be input </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>as a fraction of the chord (between 0 and 1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Ribs, Top Stringers and Bottom Stringers must be input as the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> quantity of each element per section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Leave blacked-out cells blank. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>STRINGER CROSS-SECTION TBD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The trimming of the skin and ribs must be input also as a fraction of the chord. These last inputs are included so as to prevent issues with the NASTRAN tool. </t>
-    </r>
-  </si>
-  <si>
     <t>rae5215</t>
   </si>
   <si>
@@ -594,6 +521,217 @@
   <si>
     <t>Flight Altitude [ft]</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Ribs, Top Stringers and Bottom Stringers must be input as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>quantity of each element per section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Leave blacked-out cells blank. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> The trimming of the skin and ribs must be input also as a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fraction of the chord</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. These are included so as to prevent issues with the NASTRAN tool.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The front and rear spar locations must be input as a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fraction of the chord (between 0 and 1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>Cross-sections</t>
+  </si>
+  <si>
+    <r>
+      <t>L [mm] / S [mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t [mm] / Ix [mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J [mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Iz [mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Finally, the cross section inputs are defined by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">either rectangular dimensions or a collection of moments of inertia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. To define a shape with rectangular cross section, simply write its length (L) and thickness (t). Otherwise, write its area (S), MOI in the horizontal axis (Ix), MOI in the vertical axis (Iy), and its polar moment of inertia (J).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -603,13 +741,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -651,6 +782,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -661,13 +800,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,10 +992,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -870,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -879,7 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -888,8 +1027,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -903,10 +1040,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -915,10 +1052,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -928,14 +1061,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -947,46 +1086,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1007,13 +1146,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1025,10 +1164,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1046,7 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1076,6 +1215,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1393,8 +1576,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,22 +1601,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="40"/>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1588,100 +1771,100 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="55" t="s">
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="54"/>
+      <c r="O15" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="P15" s="54"/>
+    </row>
+    <row r="16" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="N16" s="56"/>
+      <c r="O16" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="P16" s="56"/>
+    </row>
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="56"/>
-      <c r="O15" s="55" t="s">
+      <c r="N17" s="56"/>
+      <c r="O17" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="P17" s="56"/>
+    </row>
+    <row r="18" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="P15" s="56"/>
-    </row>
-    <row r="16" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="N16" s="58"/>
-      <c r="O16" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="P16" s="58"/>
-    </row>
-    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="63" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="N17" s="58"/>
-      <c r="O17" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="P17" s="58"/>
-    </row>
-    <row r="18" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="N18" s="68"/>
-      <c r="O18" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="P18" s="68"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="P18" s="66"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
@@ -1717,27 +1900,27 @@
       <c r="L20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="N20" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="O20" s="44"/>
-      <c r="P20" s="45"/>
+      <c r="N20" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="O20" s="42"/>
+      <c r="P20" s="43"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -1747,23 +1930,23 @@
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="N21" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="36">
+      <c r="B22" s="32">
         <v>0</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="32">
         <v>1</v>
       </c>
       <c r="D22" s="12">
@@ -1780,24 +1963,24 @@
       <c r="K22" s="12"/>
       <c r="L22" s="13"/>
       <c r="N22" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="O22" t="s">
         <v>23</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N23" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +2001,7 @@
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O18:P18"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1830,7 +2013,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,18 +2022,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="40" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -1879,37 +2062,37 @@
       <c r="A4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1930,7 +2113,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="33"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1950,7 +2133,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B10" s="4">
         <v>1000</v>
@@ -1961,7 +2144,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1969,826 +2152,979 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:21" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="42"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="59"/>
+    </row>
+    <row r="2" spans="1:21" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="56"/>
+    </row>
+    <row r="3" spans="1:21" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="56"/>
+    </row>
+    <row r="4" spans="1:21" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B4">
+      <c r="B7" s="5">
         <v>0.05</v>
       </c>
-      <c r="C4">
+      <c r="C7" s="8">
         <v>0.4</v>
       </c>
-      <c r="D4">
+      <c r="D7" s="8">
         <v>0.05</v>
       </c>
-      <c r="E4">
+      <c r="E7" s="8">
         <v>0.2</v>
       </c>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5">
+      <c r="B8" s="6">
         <v>0.75</v>
       </c>
-      <c r="C5">
+      <c r="C8" s="84">
         <v>0.76</v>
       </c>
-      <c r="D5">
+      <c r="D8" s="84">
         <v>0.78</v>
       </c>
-      <c r="E5">
+      <c r="E8" s="84">
         <v>0.8</v>
       </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6">
+      <c r="B9" s="100"/>
+      <c r="C9" s="84">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="D9" s="84">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E9" s="84">
         <v>3</v>
       </c>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7">
+      <c r="B10" s="100"/>
+      <c r="C10" s="84">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="D10" s="84">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="E10" s="84">
         <v>3</v>
       </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8">
+      <c r="B11" s="101"/>
+      <c r="C11" s="12">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D11" s="12">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E11" s="12">
         <v>2</v>
       </c>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B13" s="3">
         <v>0.94</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B14" s="4">
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="84"/>
+      <c r="B15" s="84"/>
+    </row>
+    <row r="16" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="84">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="D18" s="84">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2.2532999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="21" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="59" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="22" t="s">
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="N15" s="81" t="s">
+      <c r="N21" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="23" t="s">
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="80"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="72" t="s">
+      <c r="N22" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="73"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="23" t="s">
+      <c r="O22" s="70"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="71"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="47"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N17" s="72" t="s">
+      <c r="N23" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="73"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="24" t="s">
+      <c r="O23" s="70"/>
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="71"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N18" s="74" t="s">
+      <c r="N24" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="75"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
-      <c r="B20" s="76" t="s">
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="73"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="76"/>
+      <c r="B26" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="H20" s="76" t="s">
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="H26" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
-      <c r="B21" s="16" t="s">
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="76"/>
+      <c r="B27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I27" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="77" t="s">
+      <c r="J27" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="77"/>
-      <c r="L21" s="16" t="s">
+      <c r="K27" s="75"/>
+      <c r="L27" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="78"/>
-      <c r="B22" s="26" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="76"/>
+      <c r="B28" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C28" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E28" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H28" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I28" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="J28" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="K28" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B29" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C29" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D29" s="18">
         <v>1.27</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E29" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H29" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I29" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J23">
+      <c r="J29">
         <v>0.20319999999999999</v>
       </c>
-      <c r="K23">
+      <c r="K29">
         <v>0.22859999999999997</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L29" s="24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B30" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D24">
+      <c r="D30" s="30">
         <v>1.524</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E30" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H30" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I30" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J24">
+      <c r="J30">
         <v>0.20319999999999999</v>
       </c>
-      <c r="K24">
+      <c r="K30">
         <v>0.22859999999999997</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L30" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B31" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C31" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D25">
+      <c r="D31" s="30">
         <v>1.27</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E31" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H31" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I31" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J25">
+      <c r="J31">
         <v>0.254</v>
       </c>
-      <c r="K25">
+      <c r="K31">
         <v>1.5748</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L31" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B32" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C32" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D26">
+      <c r="D32" s="30">
         <v>1.524</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E32" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H32" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I32" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J26">
+      <c r="J32">
         <v>0.254</v>
       </c>
-      <c r="K26">
+      <c r="K32">
         <v>1.5748</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="L32" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B33" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C33" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D27">
+      <c r="D33" s="30">
         <v>1.27</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E33" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H33" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I33" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J27">
+      <c r="J33">
         <v>1.6001999999999998</v>
       </c>
-      <c r="K27">
+      <c r="K33">
         <v>3.2511999999999999</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="L33" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B34" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C34" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D34" s="95">
         <v>1.524</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E34" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H34" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I34" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J28">
+      <c r="J34">
         <v>1.6001999999999998</v>
       </c>
-      <c r="K28">
+      <c r="K34">
         <v>3.2511999999999999</v>
       </c>
-      <c r="L28" s="7" t="s">
+      <c r="L34" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H29" s="6" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H35" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I35" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J29">
+      <c r="J35">
         <v>3.2765999999999997</v>
       </c>
-      <c r="K29">
+      <c r="K35">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L35" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H30" s="6" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H36" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I36" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="J30">
+      <c r="J36">
         <v>3.2765999999999997</v>
       </c>
-      <c r="K30">
+      <c r="K36">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="L36" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="71"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="H31" s="6" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="H37" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I37" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J31">
+      <c r="J37">
         <v>6.35</v>
       </c>
-      <c r="K31">
+      <c r="K37">
         <v>38.099999999999994</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L37" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H32" s="6" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H38" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I38" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J32">
+      <c r="J38">
         <v>6.35</v>
       </c>
-      <c r="K32">
+      <c r="K38">
         <v>38.099999999999994</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L38" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H33" s="6" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H39" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I39" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J33">
+      <c r="J39">
         <v>38.125399999999992</v>
       </c>
-      <c r="K33">
+      <c r="K39">
         <v>50.8</v>
       </c>
-      <c r="L33" s="7" t="s">
+      <c r="L39" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H34" s="6" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H40" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I40" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J34">
+      <c r="J40">
         <v>38.125399999999992</v>
       </c>
-      <c r="K34">
+      <c r="K40">
         <v>50.8</v>
       </c>
-      <c r="L34" s="7" t="s">
+      <c r="L40" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H35" s="6" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H41" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I41" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J35">
+      <c r="J41">
         <v>50.825399999999995</v>
       </c>
-      <c r="K35">
+      <c r="K41">
         <v>76.199999999999989</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="L41" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H36" s="6" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H42" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I42" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J36">
+      <c r="J42">
         <v>50.825399999999995</v>
       </c>
-      <c r="K36">
+      <c r="K42">
         <v>76.199999999999989</v>
       </c>
-      <c r="L36" s="7" t="s">
+      <c r="L42" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H37" s="6" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H43" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I43" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J37">
+      <c r="J43">
         <v>76.225399999999993</v>
       </c>
-      <c r="K37">
+      <c r="K43">
         <v>101.6</v>
       </c>
-      <c r="L37" s="7" t="s">
+      <c r="L43" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H38" s="6" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H44" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I44" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="J38">
+      <c r="J44">
         <v>76.225399999999993</v>
       </c>
-      <c r="K38">
+      <c r="K44">
         <v>101.6</v>
       </c>
-      <c r="L38" s="7" t="s">
+      <c r="L44" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H39" s="6" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H45" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I45" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="J39">
+      <c r="J45">
         <v>1.016</v>
       </c>
-      <c r="K39">
+      <c r="K45">
         <v>1.5748</v>
       </c>
-      <c r="L39" s="7" t="s">
+      <c r="L45" s="96" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H40" s="6" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H46" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I46" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="J40">
+      <c r="J46">
         <v>1.6001999999999998</v>
       </c>
-      <c r="K40">
+      <c r="K46">
         <v>4.7497999999999996</v>
       </c>
-      <c r="L40" s="7" t="s">
+      <c r="L46" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H41" s="6" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H47" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I47" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="J41">
+      <c r="J47">
         <v>1.6001999999999998</v>
       </c>
-      <c r="K41">
+      <c r="K47">
         <v>4.7497999999999996</v>
       </c>
-      <c r="L41" s="7" t="s">
+      <c r="L47" s="96" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H42" s="11" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H48" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I48" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J48" s="12">
         <v>4.7751999999999999</v>
       </c>
-      <c r="K42" s="12">
+      <c r="K48" s="12">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="L48" s="97" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E1:R1"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A15:D18"/>
-    <mergeCell ref="E15:L18"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="N16:R16"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="E4:S4"/>
+    <mergeCell ref="E3:S3"/>
+    <mergeCell ref="E2:S2"/>
+    <mergeCell ref="E1:S1"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A21:D24"/>
+    <mergeCell ref="E21:L24"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="N22:R22"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2798,25 +3134,25 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="83" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
femfilegenerator.py now considers bcs placement.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A3E4D-B46D-492A-9D0F-F1044F8614E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="150">
   <si>
     <t>Section 1</t>
   </si>
@@ -971,12 +970,15 @@
       </rPr>
       <t>. If the root rib is clamped in a certain DOF, the other two components will be as well.</t>
     </r>
+  </si>
+  <si>
+    <t>b29_root</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1465,6 +1467,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1491,18 +1505,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1829,12 +1831,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,7 +2157,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>109</v>
@@ -2250,7 +2252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -2392,7 +2394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S48"/>
   <sheetViews>
@@ -2719,7 +2721,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="88"/>
+      <c r="D21" s="92"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2733,19 +2735,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="91" t="s">
+      <c r="N21" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="92"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="96"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="89"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2757,19 +2759,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="93"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="98"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="89"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2781,19 +2783,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="N23" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="93"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="98"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="90"/>
+      <c r="D24" s="94"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2805,32 +2807,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="95" t="s">
+      <c r="N24" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="96"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="H26" s="98" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="H26" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2849,16 +2851,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="99"/>
+      <c r="K27" s="90"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3114,10 +3116,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3323,11 +3325,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3339,6 +3336,11 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3346,12 +3348,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3374,7 +3376,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="92"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3394,7 +3396,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="89"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="80" t="s">
         <v>131</v>
       </c>
@@ -3414,7 +3416,7 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="89"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="80" t="s">
         <v>146</v>
       </c>
@@ -3434,7 +3436,7 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="89"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="80" t="s">
         <v>147</v>
       </c>
@@ -3454,7 +3456,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="89"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="80" t="s">
         <v>132</v>
       </c>
@@ -3474,7 +3476,7 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="90"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="66" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
femfilegenerator can correctly create bdf files.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D05E62C-FC34-4B7C-8FB0-9493E4A44DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -764,9 +763,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Boundary Conditions</t>
   </si>
   <si>
@@ -971,12 +967,15 @@
       </rPr>
       <t>. If the root rib is clamped in a certain DOF, the other two components will be as well.</t>
     </r>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1465,6 +1464,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1491,18 +1502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1829,12 +1828,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,7 +2249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -2392,7 +2391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S48"/>
   <sheetViews>
@@ -2719,7 +2718,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="88"/>
+      <c r="D21" s="92"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2733,19 +2732,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="91" t="s">
+      <c r="N21" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="92"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="96"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="89"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2757,19 +2756,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="93"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="98"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="89"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2781,19 +2780,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="N23" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="93"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="98"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="90"/>
+      <c r="D24" s="94"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2805,32 +2804,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="95" t="s">
+      <c r="N24" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="96"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="H26" s="98" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="H26" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2849,16 +2848,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="99"/>
+      <c r="K27" s="90"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3114,10 +3113,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3323,11 +3322,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3339,6 +3333,11 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3346,12 +3345,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3374,7 +3373,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="92"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3394,7 +3393,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="89"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="80" t="s">
         <v>131</v>
       </c>
@@ -3414,9 +3413,9 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="89"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="80" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="104"/>
       <c r="E3" s="104"/>
@@ -3434,9 +3433,9 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="89"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D4" s="104"/>
       <c r="E4" s="104"/>
@@ -3454,7 +3453,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="89"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="80" t="s">
         <v>132</v>
       </c>
@@ -3474,9 +3473,9 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="90"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" s="83"/>
       <c r="E6" s="83"/>
@@ -3522,7 +3521,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="51">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -3538,45 +3537,45 @@
         <v>130</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
@@ -3584,33 +3583,33 @@
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="54"/>
       <c r="C16" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="55"/>
       <c r="F16" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G16" s="56"/>
     </row>
     <row r="17" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="57"/>
       <c r="C17" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17" s="58"/>
       <c r="E17" s="58"/>
       <c r="F17" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G17" s="59"/>
     </row>

</xml_diff>

<commit_message>
Final commit. Project ready.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661D5EE3-A119-404F-911A-D5EA89D7DDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFE25645-CAA4-46BC-891C-C1136DA17492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="structural_details" sheetId="3" r:id="rId3"/>
     <sheet name="mesh_details" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -979,7 +978,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1468,6 +1467,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1479,33 +1505,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1829,12 +1828,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936DE62C-6E38-4FDD-8675-A15C0637C8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2194,10 +2193,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="12">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="12">
-        <v>0.7</v>
+        <v>0.8125</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -2250,7 +2249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085AC1E5-BA1E-4BD2-BFA1-56F53ABB5652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -2392,7 +2391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A908CF4-FA9E-4A63-8397-CB8EDCFE2AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S48"/>
   <sheetViews>
@@ -2720,7 +2719,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="92"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2734,19 +2733,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="95" t="s">
+      <c r="N21" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="96"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="91"/>
+      <c r="R21" s="92"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="93"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2758,19 +2757,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="97" t="s">
+      <c r="N22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="97"/>
-      <c r="P22" s="97"/>
-      <c r="Q22" s="97"/>
-      <c r="R22" s="98"/>
+      <c r="O22" s="93"/>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="93"/>
+      <c r="R22" s="94"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="93"/>
+      <c r="D23" s="89"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2782,19 +2781,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="97" t="s">
+      <c r="N23" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="97"/>
-      <c r="P23" s="97"/>
-      <c r="Q23" s="97"/>
-      <c r="R23" s="98"/>
+      <c r="O23" s="93"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="93"/>
+      <c r="R23" s="94"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="94"/>
+      <c r="D24" s="90"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2806,32 +2805,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="99" t="s">
+      <c r="N24" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="99"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="96"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="88"/>
-      <c r="B26" s="89" t="s">
+      <c r="A26" s="97"/>
+      <c r="B26" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="H26" s="89" t="s">
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="H26" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="98"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
+      <c r="A27" s="97"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2850,16 +2849,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="90" t="s">
+      <c r="J27" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="90"/>
+      <c r="K27" s="99"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="88"/>
+      <c r="A28" s="97"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3115,10 +3114,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="91"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
+      <c r="A37" s="100"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3324,6 +3323,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3335,11 +3339,6 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3347,7 +3346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310447BE-ADA4-4D16-9ACC-C2445932629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P17"/>
   <sheetViews>
@@ -3375,7 +3374,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="92"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3395,7 +3394,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="93"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="80" t="s">
         <v>130</v>
       </c>
@@ -3415,7 +3414,7 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="93"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="80" t="s">
         <v>144</v>
       </c>
@@ -3435,7 +3434,7 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="93"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="80" t="s">
         <v>145</v>
       </c>
@@ -3455,7 +3454,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="80" t="s">
         <v>131</v>
       </c>
@@ -3475,7 +3474,7 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="94"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="66" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
Big Update. requirements.txt has been updated, the App main file has been created, some small things have been modified, redundant validators have been erased.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdomi\PycharmProjects\Wingbox_w_GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73FF5AE-5311-43A2-ACD0-58E24BB8DFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
   <si>
     <t>Section 1</t>
   </si>
@@ -978,7 +979,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1467,6 +1468,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1493,18 +1506,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1828,12 +1829,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,17 +2154,17 @@
       <c r="A21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>108</v>
+      <c r="B21" s="8">
+        <v>3212</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3212</v>
       </c>
       <c r="D21" s="8">
         <v>3212</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>114</v>
+      <c r="E21" s="8">
+        <v>3212</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -2249,7 +2250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -2391,7 +2392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S48"/>
   <sheetViews>
@@ -2719,7 +2720,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="88"/>
+      <c r="D21" s="92"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2733,19 +2734,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="91" t="s">
+      <c r="N21" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="92"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="96"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="89"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2757,19 +2758,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="93"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="98"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="89"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2781,19 +2782,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="N23" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="93"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="98"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="90"/>
+      <c r="D24" s="94"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2805,32 +2806,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="95" t="s">
+      <c r="N24" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="96"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="H26" s="98" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="H26" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2849,16 +2850,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="99"/>
+      <c r="K27" s="90"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3114,10 +3115,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3323,11 +3324,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3339,6 +3335,11 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3346,7 +3347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P17"/>
   <sheetViews>
@@ -3374,7 +3375,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="92"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3394,7 +3395,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="89"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="80" t="s">
         <v>130</v>
       </c>
@@ -3414,7 +3415,7 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="89"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="80" t="s">
         <v>144</v>
       </c>
@@ -3434,7 +3435,7 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="89"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="80" t="s">
         <v>145</v>
       </c>
@@ -3454,7 +3455,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="89"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="80" t="s">
         <v>131</v>
       </c>
@@ -3474,7 +3475,7 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="90"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="66" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
NASTRAN running and output data exporting automation. Code now has only one analysis method, 'FEMAnalysis', that creates the FEM file, runs it in NASTRAN and sort output data. Input file now also has a 'NASTRAN_path' field.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\Final Assignment\kbe_wingbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profissional\Universidade\TU Delft Exchange Program\Exchange Studies\3. Third Quarter\[AE4204] Knowledge Based Engineering\KBE Competition\Wingbox_w_GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="152">
   <si>
     <t>Section 1</t>
   </si>
@@ -973,6 +973,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>NASTRAN executable file path</t>
+  </si>
+  <si>
+    <t>C:\Program Files\MSC.Software\NaPa_SE\20231\Nastran\bin\nastranw.exe</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1039,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1055,6 +1061,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1467,6 +1479,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1494,18 +1518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1514,6 +1526,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1832,7 +1853,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2719,7 +2740,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="88"/>
+      <c r="D21" s="92"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2733,19 +2754,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="91" t="s">
+      <c r="N21" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="92"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="96"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="89"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2757,19 +2778,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="93"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="98"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="89"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2781,19 +2802,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="N23" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="93"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="98"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="90"/>
+      <c r="D24" s="94"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2805,32 +2826,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="95" t="s">
+      <c r="N24" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="96"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="H26" s="98" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="H26" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2849,16 +2870,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="99"/>
+      <c r="K27" s="90"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3114,10 +3135,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3323,11 +3344,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3339,6 +3355,11 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3348,10 +3369,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3374,7 +3395,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="92"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3394,7 +3415,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="89"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="80" t="s">
         <v>130</v>
       </c>
@@ -3414,7 +3435,7 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="89"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="80" t="s">
         <v>144</v>
       </c>
@@ -3434,7 +3455,7 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="89"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="80" t="s">
         <v>145</v>
       </c>
@@ -3454,7 +3475,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="89"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="80" t="s">
         <v>131</v>
       </c>
@@ -3474,7 +3495,7 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="90"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="66" t="s">
         <v>146</v>
       </c>
@@ -3494,35 +3515,46 @@
     </row>
     <row r="8" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="103"/>
+        <v>150</v>
+      </c>
+      <c r="B8" s="104" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="106"/>
     </row>
     <row r="9" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>132</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B9" s="101"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="103"/>
     </row>
     <row r="10" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="51">
-        <v>0.1</v>
+        <v>126</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>132</v>
       </c>
       <c r="P10" t="s">
         <v>148</v>
@@ -3530,7 +3562,7 @@
     </row>
     <row r="11" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="51">
         <v>0.1</v>
@@ -3538,95 +3570,104 @@
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="51">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B13" s="50" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
+    <row r="14" spans="1:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B15" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C15" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D15" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E15" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F15" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G15" s="17" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55" t="s">
+      <c r="D16" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="56"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="56"/>
+    </row>
+    <row r="18" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58" t="s">
+      <c r="B18" s="57"/>
+      <c r="C18" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58" t="s">
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="59"/>
+      <c r="G18" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:B6"/>
-    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
     <mergeCell ref="C6:P6"/>
     <mergeCell ref="C5:P5"/>
     <mergeCell ref="C4:P4"/>
     <mergeCell ref="C3:P3"/>
     <mergeCell ref="C2:P2"/>
     <mergeCell ref="C1:P1"/>
+    <mergeCell ref="B8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Separated plots and reactions in two codes.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -1479,6 +1479,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1490,33 +1517,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
-      <c r="D21" s="92"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="77" t="s">
         <v>61</v>
       </c>
@@ -2754,19 +2754,19 @@
       <c r="M21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="95" t="s">
+      <c r="N21" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="96"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="91"/>
+      <c r="R21" s="92"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="73"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="93"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="80"/>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2778,19 +2778,19 @@
       <c r="M22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="97" t="s">
+      <c r="N22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="97"/>
-      <c r="P22" s="97"/>
-      <c r="Q22" s="97"/>
-      <c r="R22" s="98"/>
+      <c r="O22" s="93"/>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="93"/>
+      <c r="R22" s="94"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
-      <c r="D23" s="93"/>
+      <c r="D23" s="89"/>
       <c r="E23" s="80"/>
       <c r="F23" s="81"/>
       <c r="G23" s="81"/>
@@ -2802,19 +2802,19 @@
       <c r="M23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="97" t="s">
+      <c r="N23" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="97"/>
-      <c r="P23" s="97"/>
-      <c r="Q23" s="97"/>
-      <c r="R23" s="98"/>
+      <c r="O23" s="93"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="93"/>
+      <c r="R23" s="94"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="75"/>
       <c r="B24" s="76"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="94"/>
+      <c r="D24" s="90"/>
       <c r="E24" s="66"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
@@ -2826,32 +2826,32 @@
       <c r="M24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="99" t="s">
+      <c r="N24" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="99"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="96"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="88"/>
-      <c r="B26" s="89" t="s">
+      <c r="A26" s="97"/>
+      <c r="B26" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="H26" s="89" t="s">
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="H26" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="98"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
+      <c r="A27" s="97"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2870,16 +2870,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="90" t="s">
+      <c r="J27" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="90"/>
+      <c r="K27" s="99"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="88"/>
+      <c r="A28" s="97"/>
       <c r="B28" s="24" t="s">
         <v>74</v>
       </c>
@@ -3135,10 +3135,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="91"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
+      <c r="A37" s="100"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
       <c r="H37" s="42" t="s">
         <v>80</v>
       </c>
@@ -3344,6 +3344,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3355,11 +3360,6 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3395,7 +3395,7 @@
       <c r="A1" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="92"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="77" t="s">
         <v>95</v>
       </c>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73"/>
-      <c r="B2" s="93"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="80" t="s">
         <v>130</v>
       </c>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="93"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="80" t="s">
         <v>144</v>
       </c>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="93"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="80" t="s">
         <v>145</v>
       </c>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="80" t="s">
         <v>131</v>
       </c>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75"/>
-      <c r="B6" s="94"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="66" t="s">
         <v>146</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>127</v>
       </c>
       <c r="B11" s="51">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Small correction in input file.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -972,19 +972,22 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>NASTRAN executable file path</t>
   </si>
   <si>
     <t>C:\Program Files\MSC.Software\NaPa_SE\20231\Nastran\bin\nastranw.exe</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1252,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1284,9 +1287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1479,6 +1479,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1506,18 +1518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1535,6 +1535,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1853,8 +1861,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,22 +1877,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="65"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -2039,160 +2047,160 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="77" t="s">
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="84" t="s">
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="N15" s="85"/>
-      <c r="O15" s="84" t="s">
+      <c r="N15" s="84"/>
+      <c r="O15" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="P15" s="85"/>
+      <c r="P15" s="84"/>
     </row>
     <row r="16" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="80" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="N16" s="82"/>
-      <c r="O16" s="80" t="s">
+      <c r="N16" s="81"/>
+      <c r="O16" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="P16" s="82"/>
+      <c r="P16" s="81"/>
     </row>
     <row r="17" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="73"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="80" t="s">
+      <c r="A17" s="72"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="N17" s="82"/>
-      <c r="O17" s="80" t="s">
+      <c r="N17" s="81"/>
+      <c r="O17" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="82"/>
+      <c r="P17" s="81"/>
     </row>
     <row r="18" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="75"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="66" t="s">
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="N18" s="67"/>
-      <c r="O18" s="66" t="s">
+      <c r="N18" s="66"/>
+      <c r="O18" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="P18" s="67"/>
+      <c r="P18" s="66"/>
     </row>
     <row r="20" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="K20" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="24" t="s">
+      <c r="L20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="68" t="s">
+      <c r="N20" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="O20" s="69"/>
-      <c r="P20" s="70"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="69"/>
     </row>
     <row r="21" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="107">
         <v>3212</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="107" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
+      <c r="J21" s="108"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="109"/>
       <c r="N21" s="5" t="s">
         <v>107</v>
       </c>
@@ -2204,13 +2212,13 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="34">
         <v>0</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>1</v>
       </c>
       <c r="D22" s="12">
@@ -2284,18 +2292,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="63" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -2324,37 +2332,37 @@
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2375,7 +2383,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="29"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -2417,7 +2425,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,98 +2440,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="77" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="79"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="78"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="80" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="82"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="80" t="s">
+      <c r="A3" s="72"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="82"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="81"/>
     </row>
     <row r="4" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="66" t="s">
+      <c r="A4" s="74"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="67"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="66"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -2607,15 +2615,15 @@
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="35"/>
       <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
       </c>
       <c r="L9" s="10"/>
     </row>
@@ -2623,7 +2631,7 @@
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="35"/>
       <c r="C10">
         <v>7</v>
       </c>
@@ -2639,7 +2647,7 @@
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="37"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="12">
         <v>5</v>
       </c>
@@ -2662,7 +2670,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="3">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -2675,7 +2683,7 @@
     </row>
     <row r="15" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>118</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -2692,7 +2700,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>93</v>
       </c>
       <c r="B17" s="5">
@@ -2705,7 +2713,7 @@
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="6">
@@ -2722,7 +2730,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="11">
@@ -2735,123 +2743,123 @@
       <c r="E19" s="13"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="77" t="s">
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="20" t="s">
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="91" t="s">
+      <c r="N21" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="92"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="94"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="73"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="21" t="s">
+      <c r="A22" s="72"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="93"/>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="97"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="21" t="s">
+      <c r="A23" s="72"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="N23" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="93"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="94"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="97"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="75"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="22" t="s">
+      <c r="A24" s="74"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="95" t="s">
+      <c r="N24" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="96"/>
+      <c r="O24" s="98"/>
+      <c r="P24" s="98"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="99"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="87"/>
+      <c r="B26" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="H26" s="98" t="s">
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="H26" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="87"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2870,26 +2878,26 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="99"/>
+      <c r="K27" s="89"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
-      <c r="B28" s="24" t="s">
+      <c r="A28" s="87"/>
+      <c r="B28" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="23" t="s">
         <v>77</v>
       </c>
       <c r="H28" s="16" t="s">
@@ -2909,25 +2917,25 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="39" t="s">
         <v>79</v>
       </c>
       <c r="D29" s="18">
         <v>1.27</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="42" t="s">
+      <c r="H29" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I29" s="24" t="s">
+      <c r="I29" s="23" t="s">
         <v>79</v>
       </c>
       <c r="J29">
@@ -2936,30 +2944,30 @@
       <c r="K29">
         <v>0.22859999999999997</v>
       </c>
-      <c r="L29" s="24" t="s">
+      <c r="L29" s="23" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="30">
+      <c r="D30" s="29">
         <v>1.524</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="H30" s="42" t="s">
+      <c r="H30" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="43" t="s">
+      <c r="I30" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J30">
@@ -2968,30 +2976,30 @@
       <c r="K30">
         <v>0.22859999999999997</v>
       </c>
-      <c r="L30" s="43" t="s">
+      <c r="L30" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="29">
         <v>1.27</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="42" t="s">
+      <c r="H31" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I31" s="43" t="s">
+      <c r="I31" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J31">
@@ -3000,30 +3008,30 @@
       <c r="K31">
         <v>1.5748</v>
       </c>
-      <c r="L31" s="43" t="s">
+      <c r="L31" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="29">
         <v>1.524</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J32">
@@ -3032,30 +3040,30 @@
       <c r="K32">
         <v>1.5748</v>
       </c>
-      <c r="L32" s="43" t="s">
+      <c r="L32" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="29">
         <v>1.27</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J33">
@@ -3064,30 +3072,30 @@
       <c r="K33">
         <v>3.2511999999999999</v>
       </c>
-      <c r="L33" s="43" t="s">
+      <c r="L33" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="46">
+      <c r="D34" s="45">
         <v>1.524</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="42" t="s">
+      <c r="H34" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I34" s="43" t="s">
+      <c r="I34" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J34">
@@ -3096,15 +3104,15 @@
       <c r="K34">
         <v>3.2511999999999999</v>
       </c>
-      <c r="L34" s="43" t="s">
+      <c r="L34" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H35" s="42" t="s">
+      <c r="H35" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="43" t="s">
+      <c r="I35" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J35">
@@ -3113,15 +3121,15 @@
       <c r="K35">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L35" s="43" t="s">
+      <c r="L35" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H36" s="42" t="s">
+      <c r="H36" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="43" t="s">
+      <c r="I36" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J36">
@@ -3130,19 +3138,19 @@
       <c r="K36">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L36" s="43" t="s">
+      <c r="L36" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="H37" s="42" t="s">
+      <c r="A37" s="90"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="H37" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="43" t="s">
+      <c r="I37" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J37">
@@ -3151,15 +3159,15 @@
       <c r="K37">
         <v>38.099999999999994</v>
       </c>
-      <c r="L37" s="43" t="s">
+      <c r="L37" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H38" s="42" t="s">
+      <c r="H38" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I38" s="43" t="s">
+      <c r="I38" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J38">
@@ -3168,15 +3176,15 @@
       <c r="K38">
         <v>38.099999999999994</v>
       </c>
-      <c r="L38" s="43" t="s">
+      <c r="L38" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I39" s="43" t="s">
+      <c r="I39" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J39">
@@ -3185,15 +3193,15 @@
       <c r="K39">
         <v>50.8</v>
       </c>
-      <c r="L39" s="43" t="s">
+      <c r="L39" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H40" s="42" t="s">
+      <c r="H40" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I40" s="43" t="s">
+      <c r="I40" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J40">
@@ -3202,15 +3210,15 @@
       <c r="K40">
         <v>50.8</v>
       </c>
-      <c r="L40" s="43" t="s">
+      <c r="L40" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H41" s="42" t="s">
+      <c r="H41" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I41" s="43" t="s">
+      <c r="I41" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J41">
@@ -3219,15 +3227,15 @@
       <c r="K41">
         <v>76.199999999999989</v>
       </c>
-      <c r="L41" s="43" t="s">
+      <c r="L41" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H42" s="42" t="s">
+      <c r="H42" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="43" t="s">
+      <c r="I42" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J42">
@@ -3236,15 +3244,15 @@
       <c r="K42">
         <v>76.199999999999989</v>
       </c>
-      <c r="L42" s="43" t="s">
+      <c r="L42" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H43" s="42" t="s">
+      <c r="H43" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="43" t="s">
+      <c r="I43" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J43">
@@ -3253,15 +3261,15 @@
       <c r="K43">
         <v>101.6</v>
       </c>
-      <c r="L43" s="43" t="s">
+      <c r="L43" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H44" s="42" t="s">
+      <c r="H44" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I44" s="43" t="s">
+      <c r="I44" s="42" t="s">
         <v>81</v>
       </c>
       <c r="J44">
@@ -3270,15 +3278,15 @@
       <c r="K44">
         <v>101.6</v>
       </c>
-      <c r="L44" s="43" t="s">
+      <c r="L44" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I45" s="43" t="s">
+      <c r="I45" s="42" t="s">
         <v>83</v>
       </c>
       <c r="J45">
@@ -3287,15 +3295,15 @@
       <c r="K45">
         <v>1.5748</v>
       </c>
-      <c r="L45" s="43" t="s">
+      <c r="L45" s="42" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H46" s="42" t="s">
+      <c r="H46" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I46" s="43" t="s">
+      <c r="I46" s="42" t="s">
         <v>83</v>
       </c>
       <c r="J46">
@@ -3304,15 +3312,15 @@
       <c r="K46">
         <v>4.7497999999999996</v>
       </c>
-      <c r="L46" s="43" t="s">
+      <c r="L46" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H47" s="42" t="s">
+      <c r="H47" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I47" s="43" t="s">
+      <c r="I47" s="42" t="s">
         <v>83</v>
       </c>
       <c r="J47">
@@ -3321,15 +3329,15 @@
       <c r="K47">
         <v>4.7497999999999996</v>
       </c>
-      <c r="L47" s="43" t="s">
+      <c r="L47" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="48" t="s">
+      <c r="I48" s="47" t="s">
         <v>83</v>
       </c>
       <c r="J48" s="12">
@@ -3338,17 +3346,12 @@
       <c r="K48" s="12">
         <v>6.3245999999999993</v>
       </c>
-      <c r="L48" s="48" t="s">
+      <c r="L48" s="47" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A37:D37"/>
     <mergeCell ref="E3:S3"/>
     <mergeCell ref="E4:S4"/>
     <mergeCell ref="A21:D24"/>
@@ -3360,6 +3363,11 @@
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3371,7 +3379,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3392,168 +3400,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="77" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="79"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="78"/>
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="80" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="82"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81"/>
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="73"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="80" t="s">
+      <c r="A3" s="72"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="79" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="82"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="73"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="80" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="82"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="81"/>
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="80" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="82"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="66" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="67"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="66"/>
     </row>
     <row r="8" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="103" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="104" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="106"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="103"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="102"/>
     </row>
     <row r="10" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>132</v>
       </c>
       <c r="P10" t="s">
@@ -3561,32 +3569,32 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="51">
-        <v>0.01</v>
+      <c r="B11" s="50">
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="51">
+      <c r="B12" s="50">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="50" t="s">
-        <v>149</v>
+      <c r="B13" s="49" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="51" t="s">
         <v>133</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -3609,53 +3617,53 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="53"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="55" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55" t="s">
+      <c r="E17" s="54"/>
+      <c r="F17" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="56"/>
+      <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58" t="s">
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="G18" s="59"/>
+      <c r="G18" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Colormaps are now being plotted for displacements.
</commit_message>
<xml_diff>
--- a/wingbox_user_inputs.xlsx
+++ b/wingbox_user_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wing_geometry" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="152">
   <si>
     <t>Section 1</t>
   </si>
@@ -978,7 +978,7 @@
     <t>C:\Program Files\MSC.Software\NaPa_SE\20231\Nastran\bin\nastranw.exe</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1395,6 +1395,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1535,14 +1543,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,8 +1861,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1877,22 +1877,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1918,7 +1918,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1984,13 +1984,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="6">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="10"/>
     </row>
@@ -1999,13 +1999,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L10" s="10"/>
     </row>
@@ -2014,13 +2014,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L11" s="10"/>
     </row>
@@ -2032,10 +2032,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="12">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="12">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -2047,96 +2047,96 @@
       <c r="L12" s="13"/>
     </row>
     <row r="15" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="76" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="83" t="s">
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="N15" s="84"/>
-      <c r="O15" s="83" t="s">
+      <c r="N15" s="88"/>
+      <c r="O15" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="P15" s="84"/>
+      <c r="P15" s="88"/>
     </row>
     <row r="16" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="79" t="s">
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="N16" s="81"/>
-      <c r="O16" s="79" t="s">
+      <c r="N16" s="85"/>
+      <c r="O16" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="P16" s="81"/>
+      <c r="P16" s="85"/>
     </row>
     <row r="17" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="72"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="79" t="s">
+      <c r="A17" s="76"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="84"/>
+      <c r="L17" s="85"/>
+      <c r="M17" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="N17" s="81"/>
-      <c r="O17" s="79" t="s">
+      <c r="N17" s="85"/>
+      <c r="O17" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="81"/>
+      <c r="P17" s="85"/>
     </row>
     <row r="18" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="65" t="s">
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="N18" s="66"/>
-      <c r="O18" s="65" t="s">
+      <c r="N18" s="70"/>
+      <c r="O18" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="P18" s="66"/>
+      <c r="P18" s="70"/>
     </row>
     <row r="20" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
@@ -2172,35 +2172,35 @@
       <c r="L20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="67" t="s">
+      <c r="N20" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="O20" s="68"/>
-      <c r="P20" s="69"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="73"/>
     </row>
     <row r="21" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="106" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="107" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="107">
-        <v>3212</v>
-      </c>
-      <c r="E21" s="107" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="108"/>
-      <c r="L21" s="109"/>
+      <c r="B21" s="59">
+        <v>12</v>
+      </c>
+      <c r="C21" s="60">
+        <v>12</v>
+      </c>
+      <c r="D21" s="60">
+        <v>12</v>
+      </c>
+      <c r="E21" s="60">
+        <v>12</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="62"/>
       <c r="N21" s="5" t="s">
         <v>107</v>
       </c>
@@ -2282,8 +2282,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2292,18 +2292,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="62" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -2369,7 +2369,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="11">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C6" s="15">
         <v>0.2</v>
@@ -2425,7 +2425,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2440,98 +2440,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="76" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="82"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="79" t="s">
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="81"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="85"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="79" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="81"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="85"/>
     </row>
     <row r="4" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="65" t="s">
+      <c r="A4" s="78"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="66"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="70"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -2574,16 +2574,16 @@
         <v>52</v>
       </c>
       <c r="B7" s="5">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C7" s="8">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="8">
         <v>0.25</v>
       </c>
       <c r="E7" s="8">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2601,13 +2601,13 @@
         <v>0.75</v>
       </c>
       <c r="C8">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="D8">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="E8">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="L8" s="10"/>
     </row>
@@ -2617,13 +2617,13 @@
       </c>
       <c r="B9" s="35"/>
       <c r="C9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L9" s="10"/>
     </row>
@@ -2743,123 +2743,123 @@
       <c r="E19" s="13"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="76" t="s">
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="78"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="82"/>
       <c r="M21" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="94" t="s">
+      <c r="N21" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="94"/>
-      <c r="P21" s="94"/>
-      <c r="Q21" s="94"/>
-      <c r="R21" s="95"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="99"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="81"/>
+      <c r="A22" s="76"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="85"/>
       <c r="M22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="96" t="s">
+      <c r="N22" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="97"/>
+      <c r="O22" s="100"/>
+      <c r="P22" s="100"/>
+      <c r="Q22" s="100"/>
+      <c r="R22" s="101"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="72"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="81"/>
+      <c r="A23" s="76"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="85"/>
       <c r="M23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="96" t="s">
+      <c r="N23" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="97"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="100"/>
+      <c r="Q23" s="100"/>
+      <c r="R23" s="101"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="74"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="66"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="70"/>
       <c r="M24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="98" t="s">
+      <c r="N24" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="98"/>
-      <c r="P24" s="98"/>
-      <c r="Q24" s="98"/>
-      <c r="R24" s="99"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
+      <c r="R24" s="103"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="87"/>
-      <c r="B26" s="88" t="s">
+      <c r="A26" s="91"/>
+      <c r="B26" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="H26" s="88" t="s">
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="H26" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
+      <c r="A27" s="91"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
@@ -2878,16 +2878,16 @@
       <c r="I27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="89" t="s">
+      <c r="J27" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="89"/>
+      <c r="K27" s="93"/>
       <c r="L27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="87"/>
+      <c r="A28" s="91"/>
       <c r="B28" s="23" t="s">
         <v>74</v>
       </c>
@@ -3143,10 +3143,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="90"/>
-      <c r="B37" s="90"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
       <c r="H37" s="41" t="s">
         <v>80</v>
       </c>
@@ -3380,7 +3380,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3400,162 +3400,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="82"/>
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="72"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="79" t="s">
+      <c r="A2" s="76"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="81"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="85"/>
     </row>
     <row r="3" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="79" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="81"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="79" t="s">
+      <c r="A4" s="76"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="83" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="81"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="85"/>
     </row>
     <row r="5" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="79" t="s">
+      <c r="A5" s="76"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="81"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
     </row>
     <row r="6" spans="1:16" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="74"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="65" t="s">
+      <c r="A6" s="78"/>
+      <c r="B6" s="97"/>
+      <c r="C6" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="66"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="70"/>
     </row>
     <row r="8" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="105"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="109"/>
     </row>
     <row r="9" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="102"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="106"/>
     </row>
     <row r="10" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
@@ -3573,7 +3573,7 @@
         <v>127</v>
       </c>
       <c r="B11" s="50">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>